<commit_message>
GUI and README fixes
</commit_message>
<xml_diff>
--- a/export/export.xlsx
+++ b/export/export.xlsx
@@ -471,7 +471,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1137</v>
+        <v>257</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>44927</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>1136</v>
+        <v>256</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>44928</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>1134</v>
+        <v>254</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>44928</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>1135</v>
+        <v>255</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>44928</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>1132</v>
+        <v>252</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>44929</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>1133</v>
+        <v>253</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>44929</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>1131</v>
+        <v>251</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>44930</v>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>1130</v>
+        <v>250</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>44931</v>
@@ -1928,7 +1928,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>1129</v>
+        <v>249</v>
       </c>
       <c r="B49" s="2" t="n">
         <v>44935</v>
@@ -2238,7 +2238,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>1127</v>
+        <v>247</v>
       </c>
       <c r="B59" s="2" t="n">
         <v>44937</v>
@@ -2269,7 +2269,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>1128</v>
+        <v>248</v>
       </c>
       <c r="B60" s="2" t="n">
         <v>44937</v>
@@ -2300,7 +2300,7 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>1125</v>
+        <v>245</v>
       </c>
       <c r="B61" s="2" t="n">
         <v>44937</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>1126</v>
+        <v>246</v>
       </c>
       <c r="B62" s="2" t="n">
         <v>44937</v>
@@ -2362,7 +2362,7 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>1124</v>
+        <v>244</v>
       </c>
       <c r="B63" s="2" t="n">
         <v>44938</v>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>1123</v>
+        <v>243</v>
       </c>
       <c r="B71" s="2" t="n">
         <v>44940</v>
@@ -2641,7 +2641,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>1122</v>
+        <v>242</v>
       </c>
       <c r="B72" s="2" t="n">
         <v>44940</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>1121</v>
+        <v>241</v>
       </c>
       <c r="B76" s="2" t="n">
         <v>44941</v>
@@ -2796,7 +2796,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>1120</v>
+        <v>240</v>
       </c>
       <c r="B77" s="2" t="n">
         <v>44942</v>
@@ -3137,7 +3137,7 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>1119</v>
+        <v>239</v>
       </c>
       <c r="B88" s="2" t="n">
         <v>44944</v>
@@ -3509,7 +3509,7 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>1118</v>
+        <v>238</v>
       </c>
       <c r="B100" s="2" t="n">
         <v>44945</v>
@@ -3540,7 +3540,7 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>1117</v>
+        <v>237</v>
       </c>
       <c r="B101" s="2" t="n">
         <v>44945</v>
@@ -3819,7 +3819,7 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>1116</v>
+        <v>236</v>
       </c>
       <c r="B110" s="2" t="n">
         <v>44947</v>
@@ -3974,7 +3974,7 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>1114</v>
+        <v>234</v>
       </c>
       <c r="B115" s="2" t="n">
         <v>44948</v>
@@ -4005,7 +4005,7 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>1115</v>
+        <v>235</v>
       </c>
       <c r="B116" s="2" t="n">
         <v>44948</v>
@@ -4439,7 +4439,7 @@
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>1106</v>
+        <v>226</v>
       </c>
       <c r="B130" s="2" t="n">
         <v>44950</v>
@@ -4470,7 +4470,7 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>1113</v>
+        <v>233</v>
       </c>
       <c r="B131" s="2" t="n">
         <v>44950</v>
@@ -4501,7 +4501,7 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>1112</v>
+        <v>232</v>
       </c>
       <c r="B132" s="2" t="n">
         <v>44950</v>
@@ -4656,7 +4656,7 @@
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>1109</v>
+        <v>229</v>
       </c>
       <c r="B137" s="2" t="n">
         <v>44951</v>
@@ -4687,7 +4687,7 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>1111</v>
+        <v>231</v>
       </c>
       <c r="B138" s="2" t="n">
         <v>44951</v>
@@ -4718,7 +4718,7 @@
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>1110</v>
+        <v>230</v>
       </c>
       <c r="B139" s="2" t="n">
         <v>44951</v>
@@ -4780,7 +4780,7 @@
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>1107</v>
+        <v>227</v>
       </c>
       <c r="B141" s="2" t="n">
         <v>44952</v>
@@ -4811,7 +4811,7 @@
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>1108</v>
+        <v>228</v>
       </c>
       <c r="B142" s="2" t="n">
         <v>44952</v>
@@ -5090,7 +5090,7 @@
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
-        <v>1105</v>
+        <v>225</v>
       </c>
       <c r="B151" s="2" t="n">
         <v>44953</v>
@@ -5462,7 +5462,7 @@
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
-        <v>1104</v>
+        <v>224</v>
       </c>
       <c r="B163" s="2" t="n">
         <v>44955</v>
@@ -5958,7 +5958,7 @@
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
-        <v>1103</v>
+        <v>223</v>
       </c>
       <c r="B179" s="2" t="n">
         <v>44956</v>
@@ -5989,7 +5989,7 @@
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
-        <v>1099</v>
+        <v>219</v>
       </c>
       <c r="B180" s="2" t="n">
         <v>44957</v>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
-        <v>1100</v>
+        <v>220</v>
       </c>
       <c r="B181" s="2" t="n">
         <v>44957</v>
@@ -6051,7 +6051,7 @@
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
-        <v>1101</v>
+        <v>221</v>
       </c>
       <c r="B182" s="2" t="n">
         <v>44957</v>
@@ -6082,7 +6082,7 @@
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
-        <v>1102</v>
+        <v>222</v>
       </c>
       <c r="B183" s="2" t="n">
         <v>44957</v>
@@ -6144,7 +6144,7 @@
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
-        <v>1096</v>
+        <v>216</v>
       </c>
       <c r="B185" s="2" t="n">
         <v>44957</v>
@@ -6237,7 +6237,7 @@
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
-        <v>1097</v>
+        <v>217</v>
       </c>
       <c r="B188" s="2" t="n">
         <v>44958</v>
@@ -6268,7 +6268,7 @@
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
-        <v>1098</v>
+        <v>218</v>
       </c>
       <c r="B189" s="2" t="n">
         <v>44958</v>
@@ -6392,7 +6392,7 @@
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
-        <v>1095</v>
+        <v>215</v>
       </c>
       <c r="B193" s="2" t="n">
         <v>44961</v>
@@ -6423,7 +6423,7 @@
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
-        <v>1094</v>
+        <v>214</v>
       </c>
       <c r="B194" s="2" t="n">
         <v>44961</v>
@@ -6826,7 +6826,7 @@
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
-        <v>1092</v>
+        <v>212</v>
       </c>
       <c r="B207" s="2" t="n">
         <v>44963</v>
@@ -6857,7 +6857,7 @@
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
-        <v>1093</v>
+        <v>213</v>
       </c>
       <c r="B208" s="2" t="n">
         <v>44963</v>
@@ -7012,7 +7012,7 @@
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
-        <v>1090</v>
+        <v>210</v>
       </c>
       <c r="B213" s="2" t="n">
         <v>44964</v>
@@ -7043,7 +7043,7 @@
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
-        <v>1091</v>
+        <v>211</v>
       </c>
       <c r="B214" s="2" t="n">
         <v>44964</v>
@@ -7136,7 +7136,7 @@
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
-        <v>1089</v>
+        <v>209</v>
       </c>
       <c r="B217" s="2" t="n">
         <v>44964</v>
@@ -7167,7 +7167,7 @@
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
-        <v>1088</v>
+        <v>208</v>
       </c>
       <c r="B218" s="2" t="n">
         <v>44964</v>
@@ -7291,7 +7291,7 @@
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
-        <v>1087</v>
+        <v>207</v>
       </c>
       <c r="B222" s="2" t="n">
         <v>44966</v>
@@ -7384,7 +7384,7 @@
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
-        <v>1086</v>
+        <v>206</v>
       </c>
       <c r="B225" s="2" t="n">
         <v>44967</v>
@@ -7413,7 +7413,7 @@
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
-        <v>1085</v>
+        <v>205</v>
       </c>
       <c r="B226" s="2" t="n">
         <v>44967</v>
@@ -7723,7 +7723,7 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
-        <v>1084</v>
+        <v>204</v>
       </c>
       <c r="B236" s="2" t="n">
         <v>44971</v>
@@ -7816,7 +7816,7 @@
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
-        <v>1082</v>
+        <v>202</v>
       </c>
       <c r="B239" s="2" t="n">
         <v>44972</v>
@@ -7847,7 +7847,7 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
-        <v>1083</v>
+        <v>203</v>
       </c>
       <c r="B240" s="2" t="n">
         <v>44972</v>
@@ -7940,7 +7940,7 @@
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
-        <v>1081</v>
+        <v>201</v>
       </c>
       <c r="B243" s="2" t="n">
         <v>44973</v>
@@ -8002,7 +8002,7 @@
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
-        <v>1080</v>
+        <v>200</v>
       </c>
       <c r="B245" s="2" t="n">
         <v>44974</v>
@@ -8157,7 +8157,7 @@
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>1079</v>
+        <v>199</v>
       </c>
       <c r="B250" s="2" t="n">
         <v>44976</v>
@@ -8188,7 +8188,7 @@
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>1077</v>
+        <v>197</v>
       </c>
       <c r="B251" s="2" t="n">
         <v>44976</v>
@@ -8250,7 +8250,7 @@
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>1078</v>
+        <v>198</v>
       </c>
       <c r="B253" s="2" t="n">
         <v>44976</v>
@@ -8281,7 +8281,7 @@
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
-        <v>1074</v>
+        <v>194</v>
       </c>
       <c r="B254" s="2" t="n">
         <v>44977</v>
@@ -8405,7 +8405,7 @@
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
-        <v>1076</v>
+        <v>196</v>
       </c>
       <c r="B258" s="2" t="n">
         <v>44977</v>
@@ -8436,7 +8436,7 @@
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
-        <v>1075</v>
+        <v>195</v>
       </c>
       <c r="B259" s="2" t="n">
         <v>44978</v>
@@ -8591,7 +8591,7 @@
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
-        <v>1071</v>
+        <v>191</v>
       </c>
       <c r="B264" s="2" t="n">
         <v>44978</v>
@@ -8715,7 +8715,7 @@
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
-        <v>1070</v>
+        <v>190</v>
       </c>
       <c r="B268" s="2" t="n">
         <v>44979</v>
@@ -8746,7 +8746,7 @@
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
-        <v>1073</v>
+        <v>193</v>
       </c>
       <c r="B269" s="2" t="n">
         <v>44979</v>
@@ -8839,7 +8839,7 @@
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
-        <v>1072</v>
+        <v>192</v>
       </c>
       <c r="B272" s="2" t="n">
         <v>44980</v>
@@ -8870,7 +8870,7 @@
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
-        <v>1066</v>
+        <v>186</v>
       </c>
       <c r="B273" s="2" t="n">
         <v>44980</v>
@@ -8963,7 +8963,7 @@
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
-        <v>1065</v>
+        <v>185</v>
       </c>
       <c r="B276" s="2" t="n">
         <v>44980</v>
@@ -8994,7 +8994,7 @@
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
-        <v>1067</v>
+        <v>187</v>
       </c>
       <c r="B277" s="2" t="n">
         <v>44981</v>
@@ -9149,7 +9149,7 @@
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
-        <v>1069</v>
+        <v>189</v>
       </c>
       <c r="B282" s="2" t="n">
         <v>44981</v>
@@ -9180,7 +9180,7 @@
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
-        <v>1068</v>
+        <v>188</v>
       </c>
       <c r="B283" s="2" t="n">
         <v>44981</v>
@@ -9490,7 +9490,7 @@
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
-        <v>1056</v>
+        <v>176</v>
       </c>
       <c r="B293" s="2" t="n">
         <v>44984</v>
@@ -9521,7 +9521,7 @@
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
-        <v>1062</v>
+        <v>182</v>
       </c>
       <c r="B294" s="2" t="n">
         <v>44984</v>
@@ -9552,7 +9552,7 @@
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
-        <v>1063</v>
+        <v>183</v>
       </c>
       <c r="B295" s="2" t="n">
         <v>44984</v>
@@ -9707,7 +9707,7 @@
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
-        <v>1064</v>
+        <v>184</v>
       </c>
       <c r="B300" s="2" t="n">
         <v>44984</v>
@@ -9769,7 +9769,7 @@
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
-        <v>1058</v>
+        <v>178</v>
       </c>
       <c r="B302" s="2" t="n">
         <v>44985</v>
@@ -9800,7 +9800,7 @@
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
-        <v>1057</v>
+        <v>177</v>
       </c>
       <c r="B303" s="2" t="n">
         <v>44985</v>
@@ -9831,7 +9831,7 @@
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
-        <v>1061</v>
+        <v>181</v>
       </c>
       <c r="B304" s="2" t="n">
         <v>44985</v>
@@ -9862,7 +9862,7 @@
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
-        <v>1053</v>
+        <v>173</v>
       </c>
       <c r="B305" s="2" t="n">
         <v>44985</v>
@@ -9893,7 +9893,7 @@
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
-        <v>1052</v>
+        <v>172</v>
       </c>
       <c r="B306" s="2" t="n">
         <v>44985</v>
@@ -9955,7 +9955,7 @@
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
-        <v>1060</v>
+        <v>180</v>
       </c>
       <c r="B308" s="2" t="n">
         <v>44985</v>
@@ -9986,7 +9986,7 @@
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
-        <v>1059</v>
+        <v>179</v>
       </c>
       <c r="B309" s="2" t="n">
         <v>44985</v>
@@ -10079,7 +10079,7 @@
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
-        <v>1050</v>
+        <v>170</v>
       </c>
       <c r="B312" s="2" t="n">
         <v>44986</v>
@@ -10172,7 +10172,7 @@
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
-        <v>1054</v>
+        <v>174</v>
       </c>
       <c r="B315" s="2" t="n">
         <v>44986</v>
@@ -10203,7 +10203,7 @@
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
-        <v>1055</v>
+        <v>175</v>
       </c>
       <c r="B316" s="2" t="n">
         <v>44986</v>
@@ -10296,7 +10296,7 @@
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
-        <v>1051</v>
+        <v>171</v>
       </c>
       <c r="B319" s="2" t="n">
         <v>44986</v>
@@ -10947,7 +10947,7 @@
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
-        <v>1049</v>
+        <v>169</v>
       </c>
       <c r="B340" s="2" t="n">
         <v>44992</v>
@@ -10976,7 +10976,7 @@
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
-        <v>1048</v>
+        <v>168</v>
       </c>
       <c r="B341" s="2" t="n">
         <v>44992</v>
@@ -11007,7 +11007,7 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
-        <v>1047</v>
+        <v>167</v>
       </c>
       <c r="B342" s="2" t="n">
         <v>44992</v>
@@ -11224,7 +11224,7 @@
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
-        <v>1045</v>
+        <v>165</v>
       </c>
       <c r="B349" s="2" t="n">
         <v>44993</v>
@@ -11255,7 +11255,7 @@
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
-        <v>1046</v>
+        <v>166</v>
       </c>
       <c r="B350" s="2" t="n">
         <v>44993</v>
@@ -11317,7 +11317,7 @@
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
-        <v>1044</v>
+        <v>164</v>
       </c>
       <c r="B352" s="2" t="n">
         <v>44994</v>
@@ -11813,7 +11813,7 @@
     </row>
     <row r="368">
       <c r="A368" s="1" t="n">
-        <v>1040</v>
+        <v>160</v>
       </c>
       <c r="B368" s="2" t="n">
         <v>45001</v>
@@ -11906,7 +11906,7 @@
     </row>
     <row r="371">
       <c r="A371" s="1" t="n">
-        <v>1043</v>
+        <v>163</v>
       </c>
       <c r="B371" s="2" t="n">
         <v>45001</v>
@@ -12030,7 +12030,7 @@
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
-        <v>1041</v>
+        <v>161</v>
       </c>
       <c r="B375" s="2" t="n">
         <v>45002</v>
@@ -12061,7 +12061,7 @@
     </row>
     <row r="376">
       <c r="A376" s="1" t="n">
-        <v>1042</v>
+        <v>162</v>
       </c>
       <c r="B376" s="2" t="n">
         <v>45002</v>
@@ -12154,7 +12154,7 @@
     </row>
     <row r="379">
       <c r="A379" s="1" t="n">
-        <v>1039</v>
+        <v>159</v>
       </c>
       <c r="B379" s="2" t="n">
         <v>45003</v>
@@ -12464,7 +12464,7 @@
     </row>
     <row r="389">
       <c r="A389" s="1" t="n">
-        <v>1037</v>
+        <v>157</v>
       </c>
       <c r="B389" s="2" t="n">
         <v>45006</v>
@@ -12495,7 +12495,7 @@
     </row>
     <row r="390">
       <c r="A390" s="1" t="n">
-        <v>1038</v>
+        <v>158</v>
       </c>
       <c r="B390" s="2" t="n">
         <v>45006</v>
@@ -12772,7 +12772,7 @@
     </row>
     <row r="399">
       <c r="A399" s="1" t="n">
-        <v>1036</v>
+        <v>156</v>
       </c>
       <c r="B399" s="2" t="n">
         <v>45008</v>
@@ -13020,7 +13020,7 @@
     </row>
     <row r="407">
       <c r="A407" s="1" t="n">
-        <v>1035</v>
+        <v>155</v>
       </c>
       <c r="B407" s="2" t="n">
         <v>45009</v>
@@ -13082,7 +13082,7 @@
     </row>
     <row r="409">
       <c r="A409" s="1" t="n">
-        <v>1034</v>
+        <v>154</v>
       </c>
       <c r="B409" s="2" t="n">
         <v>45009</v>
@@ -13113,7 +13113,7 @@
     </row>
     <row r="410">
       <c r="A410" s="1" t="n">
-        <v>1032</v>
+        <v>152</v>
       </c>
       <c r="B410" s="2" t="n">
         <v>45009</v>
@@ -13175,7 +13175,7 @@
     </row>
     <row r="412">
       <c r="A412" s="1" t="n">
-        <v>1033</v>
+        <v>153</v>
       </c>
       <c r="B412" s="2" t="n">
         <v>45009</v>
@@ -13423,7 +13423,7 @@
     </row>
     <row r="420">
       <c r="A420" s="1" t="n">
-        <v>1031</v>
+        <v>151</v>
       </c>
       <c r="B420" s="2" t="n">
         <v>45012</v>
@@ -13454,7 +13454,7 @@
     </row>
     <row r="421">
       <c r="A421" s="1" t="n">
-        <v>1029</v>
+        <v>149</v>
       </c>
       <c r="B421" s="2" t="n">
         <v>45012</v>
@@ -13609,7 +13609,7 @@
     </row>
     <row r="426">
       <c r="A426" s="1" t="n">
-        <v>1030</v>
+        <v>150</v>
       </c>
       <c r="B426" s="2" t="n">
         <v>45012</v>
@@ -13640,7 +13640,7 @@
     </row>
     <row r="427">
       <c r="A427" s="1" t="n">
-        <v>1028</v>
+        <v>148</v>
       </c>
       <c r="B427" s="2" t="n">
         <v>45013</v>
@@ -14105,7 +14105,7 @@
     </row>
     <row r="442">
       <c r="A442" s="1" t="n">
-        <v>1027</v>
+        <v>147</v>
       </c>
       <c r="B442" s="2" t="n">
         <v>45016</v>
@@ -14260,7 +14260,7 @@
     </row>
     <row r="447">
       <c r="A447" s="1" t="n">
-        <v>1023</v>
+        <v>143</v>
       </c>
       <c r="B447" s="2" t="n">
         <v>45016</v>
@@ -14291,7 +14291,7 @@
     </row>
     <row r="448">
       <c r="A448" s="1" t="n">
-        <v>1024</v>
+        <v>144</v>
       </c>
       <c r="B448" s="2" t="n">
         <v>45016</v>
@@ -14322,7 +14322,7 @@
     </row>
     <row r="449">
       <c r="A449" s="1" t="n">
-        <v>1025</v>
+        <v>145</v>
       </c>
       <c r="B449" s="2" t="n">
         <v>45016</v>
@@ -14353,7 +14353,7 @@
     </row>
     <row r="450">
       <c r="A450" s="1" t="n">
-        <v>1026</v>
+        <v>146</v>
       </c>
       <c r="B450" s="2" t="n">
         <v>45016</v>
@@ -14663,7 +14663,7 @@
     </row>
     <row r="460">
       <c r="A460" s="1" t="n">
-        <v>1022</v>
+        <v>142</v>
       </c>
       <c r="B460" s="2" t="n">
         <v>45019</v>
@@ -14694,7 +14694,7 @@
     </row>
     <row r="461">
       <c r="A461" s="1" t="n">
-        <v>1021</v>
+        <v>141</v>
       </c>
       <c r="B461" s="2" t="n">
         <v>45019</v>
@@ -14973,7 +14973,7 @@
     </row>
     <row r="470">
       <c r="A470" s="1" t="n">
-        <v>1020</v>
+        <v>140</v>
       </c>
       <c r="B470" s="2" t="n">
         <v>45021</v>
@@ -15128,7 +15128,7 @@
     </row>
     <row r="475">
       <c r="A475" s="1" t="n">
-        <v>1019</v>
+        <v>139</v>
       </c>
       <c r="B475" s="2" t="n">
         <v>45022</v>
@@ -15221,7 +15221,7 @@
     </row>
     <row r="478">
       <c r="A478" s="1" t="n">
-        <v>1018</v>
+        <v>138</v>
       </c>
       <c r="B478" s="2" t="n">
         <v>45023</v>
@@ -16616,7 +16616,7 @@
     </row>
     <row r="523">
       <c r="A523" s="1" t="n">
-        <v>1017</v>
+        <v>137</v>
       </c>
       <c r="B523" s="2" t="n">
         <v>45033</v>
@@ -17019,7 +17019,7 @@
     </row>
     <row r="536">
       <c r="A536" s="1" t="n">
-        <v>1015</v>
+        <v>135</v>
       </c>
       <c r="B536" s="2" t="n">
         <v>45037</v>
@@ -17143,7 +17143,7 @@
     </row>
     <row r="540">
       <c r="A540" s="1" t="n">
-        <v>1016</v>
+        <v>136</v>
       </c>
       <c r="B540" s="2" t="n">
         <v>45037</v>
@@ -17174,7 +17174,7 @@
     </row>
     <row r="541">
       <c r="A541" s="1" t="n">
-        <v>1014</v>
+        <v>134</v>
       </c>
       <c r="B541" s="2" t="n">
         <v>45037</v>
@@ -17236,7 +17236,7 @@
     </row>
     <row r="543">
       <c r="A543" s="1" t="n">
-        <v>1012</v>
+        <v>132</v>
       </c>
       <c r="B543" s="2" t="n">
         <v>45039</v>
@@ -17267,7 +17267,7 @@
     </row>
     <row r="544">
       <c r="A544" s="1" t="n">
-        <v>1011</v>
+        <v>131</v>
       </c>
       <c r="B544" s="2" t="n">
         <v>45039</v>
@@ -17329,7 +17329,7 @@
     </row>
     <row r="546">
       <c r="A546" s="1" t="n">
-        <v>1010</v>
+        <v>130</v>
       </c>
       <c r="B546" s="2" t="n">
         <v>45040</v>
@@ -17360,7 +17360,7 @@
     </row>
     <row r="547">
       <c r="A547" s="1" t="n">
-        <v>1013</v>
+        <v>133</v>
       </c>
       <c r="B547" s="2" t="n">
         <v>45040</v>
@@ -17391,7 +17391,7 @@
     </row>
     <row r="548">
       <c r="A548" s="1" t="n">
-        <v>1008</v>
+        <v>128</v>
       </c>
       <c r="B548" s="2" t="n">
         <v>45040</v>
@@ -17422,7 +17422,7 @@
     </row>
     <row r="549">
       <c r="A549" s="1" t="n">
-        <v>1007</v>
+        <v>127</v>
       </c>
       <c r="B549" s="2" t="n">
         <v>45040</v>
@@ -17484,7 +17484,7 @@
     </row>
     <row r="551">
       <c r="A551" s="1" t="n">
-        <v>1009</v>
+        <v>129</v>
       </c>
       <c r="B551" s="2" t="n">
         <v>45041</v>
@@ -17546,7 +17546,7 @@
     </row>
     <row r="553">
       <c r="A553" s="1" t="n">
-        <v>1005</v>
+        <v>125</v>
       </c>
       <c r="B553" s="2" t="n">
         <v>45041</v>
@@ -17577,7 +17577,7 @@
     </row>
     <row r="554">
       <c r="A554" s="1" t="n">
-        <v>1002</v>
+        <v>122</v>
       </c>
       <c r="B554" s="2" t="n">
         <v>45041</v>
@@ -17639,7 +17639,7 @@
     </row>
     <row r="556">
       <c r="A556" s="1" t="n">
-        <v>1006</v>
+        <v>126</v>
       </c>
       <c r="B556" s="2" t="n">
         <v>45041</v>
@@ -17732,7 +17732,7 @@
     </row>
     <row r="559">
       <c r="A559" s="1" t="n">
-        <v>1001</v>
+        <v>121</v>
       </c>
       <c r="B559" s="2" t="n">
         <v>45042</v>
@@ -17794,7 +17794,7 @@
     </row>
     <row r="561">
       <c r="A561" s="1" t="n">
-        <v>1003</v>
+        <v>123</v>
       </c>
       <c r="B561" s="2" t="n">
         <v>45042</v>
@@ -17825,7 +17825,7 @@
     </row>
     <row r="562">
       <c r="A562" s="1" t="n">
-        <v>1004</v>
+        <v>124</v>
       </c>
       <c r="B562" s="2" t="n">
         <v>45042</v>
@@ -18290,7 +18290,7 @@
     </row>
     <row r="577">
       <c r="A577" s="1" t="n">
-        <v>1000</v>
+        <v>120</v>
       </c>
       <c r="B577" s="2" t="n">
         <v>45043</v>
@@ -18383,7 +18383,7 @@
     </row>
     <row r="580">
       <c r="A580" s="1" t="n">
-        <v>997</v>
+        <v>117</v>
       </c>
       <c r="B580" s="2" t="n">
         <v>45044</v>
@@ -18414,7 +18414,7 @@
     </row>
     <row r="581">
       <c r="A581" s="1" t="n">
-        <v>996</v>
+        <v>116</v>
       </c>
       <c r="B581" s="2" t="n">
         <v>45044</v>
@@ -18445,7 +18445,7 @@
     </row>
     <row r="582">
       <c r="A582" s="1" t="n">
-        <v>995</v>
+        <v>115</v>
       </c>
       <c r="B582" s="2" t="n">
         <v>45044</v>
@@ -18476,7 +18476,7 @@
     </row>
     <row r="583">
       <c r="A583" s="1" t="n">
-        <v>994</v>
+        <v>114</v>
       </c>
       <c r="B583" s="2" t="n">
         <v>45044</v>
@@ -18507,7 +18507,7 @@
     </row>
     <row r="584">
       <c r="A584" s="1" t="n">
-        <v>998</v>
+        <v>118</v>
       </c>
       <c r="B584" s="2" t="n">
         <v>45044</v>
@@ -18538,7 +18538,7 @@
     </row>
     <row r="585">
       <c r="A585" s="1" t="n">
-        <v>999</v>
+        <v>119</v>
       </c>
       <c r="B585" s="2" t="n">
         <v>45044</v>
@@ -19065,7 +19065,7 @@
     </row>
     <row r="602">
       <c r="A602" s="1" t="n">
-        <v>993</v>
+        <v>113</v>
       </c>
       <c r="B602" s="2" t="n">
         <v>45048</v>
@@ -19096,7 +19096,7 @@
     </row>
     <row r="603">
       <c r="A603" s="1" t="n">
-        <v>992</v>
+        <v>112</v>
       </c>
       <c r="B603" s="2" t="n">
         <v>45048</v>
@@ -19282,7 +19282,7 @@
     </row>
     <row r="609">
       <c r="A609" s="1" t="n">
-        <v>991</v>
+        <v>111</v>
       </c>
       <c r="B609" s="2" t="n">
         <v>45050</v>
@@ -19964,7 +19964,7 @@
     </row>
     <row r="631">
       <c r="A631" s="1" t="n">
-        <v>989</v>
+        <v>109</v>
       </c>
       <c r="B631" s="2" t="n">
         <v>45058</v>
@@ -20150,7 +20150,7 @@
     </row>
     <row r="637">
       <c r="A637" s="1" t="n">
-        <v>990</v>
+        <v>110</v>
       </c>
       <c r="B637" s="2" t="n">
         <v>45058</v>
@@ -21049,7 +21049,7 @@
     </row>
     <row r="666">
       <c r="A666" s="1" t="n">
-        <v>988</v>
+        <v>108</v>
       </c>
       <c r="B666" s="2" t="n">
         <v>45067</v>
@@ -21080,7 +21080,7 @@
     </row>
     <row r="667">
       <c r="A667" s="1" t="n">
-        <v>987</v>
+        <v>107</v>
       </c>
       <c r="B667" s="2" t="n">
         <v>45068</v>
@@ -21111,7 +21111,7 @@
     </row>
     <row r="668">
       <c r="A668" s="1" t="n">
-        <v>986</v>
+        <v>106</v>
       </c>
       <c r="B668" s="2" t="n">
         <v>45068</v>
@@ -21266,7 +21266,7 @@
     </row>
     <row r="673">
       <c r="A673" s="1" t="n">
-        <v>984</v>
+        <v>104</v>
       </c>
       <c r="B673" s="2" t="n">
         <v>45069</v>
@@ -21359,7 +21359,7 @@
     </row>
     <row r="676">
       <c r="A676" s="1" t="n">
-        <v>985</v>
+        <v>105</v>
       </c>
       <c r="B676" s="2" t="n">
         <v>45070</v>
@@ -21390,7 +21390,7 @@
     </row>
     <row r="677">
       <c r="A677" s="1" t="n">
-        <v>983</v>
+        <v>103</v>
       </c>
       <c r="B677" s="2" t="n">
         <v>45070</v>
@@ -21731,7 +21731,7 @@
     </row>
     <row r="688">
       <c r="A688" s="1" t="n">
-        <v>979</v>
+        <v>99</v>
       </c>
       <c r="B688" s="2" t="n">
         <v>45071</v>
@@ -21762,7 +21762,7 @@
     </row>
     <row r="689">
       <c r="A689" s="1" t="n">
-        <v>982</v>
+        <v>102</v>
       </c>
       <c r="B689" s="2" t="n">
         <v>45072</v>
@@ -21886,7 +21886,7 @@
     </row>
     <row r="693">
       <c r="A693" s="1" t="n">
-        <v>980</v>
+        <v>100</v>
       </c>
       <c r="B693" s="2" t="n">
         <v>45072</v>
@@ -22041,7 +22041,7 @@
     </row>
     <row r="698">
       <c r="A698" s="1" t="n">
-        <v>981</v>
+        <v>101</v>
       </c>
       <c r="B698" s="2" t="n">
         <v>45072</v>
@@ -22134,7 +22134,7 @@
     </row>
     <row r="701">
       <c r="A701" s="1" t="n">
-        <v>978</v>
+        <v>98</v>
       </c>
       <c r="B701" s="2" t="n">
         <v>45073</v>
@@ -22320,7 +22320,7 @@
     </row>
     <row r="707">
       <c r="A707" s="1" t="n">
-        <v>976</v>
+        <v>96</v>
       </c>
       <c r="B707" s="2" t="n">
         <v>45075</v>
@@ -22413,7 +22413,7 @@
     </row>
     <row r="710">
       <c r="A710" s="1" t="n">
-        <v>977</v>
+        <v>97</v>
       </c>
       <c r="B710" s="2" t="n">
         <v>45075</v>
@@ -22475,7 +22475,7 @@
     </row>
     <row r="712">
       <c r="A712" s="1" t="n">
-        <v>975</v>
+        <v>95</v>
       </c>
       <c r="B712" s="2" t="n">
         <v>45077</v>
@@ -22506,7 +22506,7 @@
     </row>
     <row r="713">
       <c r="A713" s="1" t="n">
-        <v>974</v>
+        <v>94</v>
       </c>
       <c r="B713" s="2" t="n">
         <v>45077</v>
@@ -22599,7 +22599,7 @@
     </row>
     <row r="716">
       <c r="A716" s="1" t="n">
-        <v>973</v>
+        <v>93</v>
       </c>
       <c r="B716" s="2" t="n">
         <v>45077</v>
@@ -22630,7 +22630,7 @@
     </row>
     <row r="717">
       <c r="A717" s="1" t="n">
-        <v>972</v>
+        <v>92</v>
       </c>
       <c r="B717" s="2" t="n">
         <v>45077</v>
@@ -22661,7 +22661,7 @@
     </row>
     <row r="718">
       <c r="A718" s="1" t="n">
-        <v>969</v>
+        <v>89</v>
       </c>
       <c r="B718" s="2" t="n">
         <v>45077</v>
@@ -22692,7 +22692,7 @@
     </row>
     <row r="719">
       <c r="A719" s="1" t="n">
-        <v>971</v>
+        <v>91</v>
       </c>
       <c r="B719" s="2" t="n">
         <v>45078</v>
@@ -22723,7 +22723,7 @@
     </row>
     <row r="720">
       <c r="A720" s="1" t="n">
-        <v>970</v>
+        <v>90</v>
       </c>
       <c r="B720" s="2" t="n">
         <v>45078</v>
@@ -22754,7 +22754,7 @@
     </row>
     <row r="721">
       <c r="A721" s="1" t="n">
-        <v>966</v>
+        <v>86</v>
       </c>
       <c r="B721" s="2" t="n">
         <v>45078</v>
@@ -22785,7 +22785,7 @@
     </row>
     <row r="722">
       <c r="A722" s="1" t="n">
-        <v>967</v>
+        <v>87</v>
       </c>
       <c r="B722" s="2" t="n">
         <v>45078</v>
@@ -22909,7 +22909,7 @@
     </row>
     <row r="726">
       <c r="A726" s="1" t="n">
-        <v>968</v>
+        <v>88</v>
       </c>
       <c r="B726" s="2" t="n">
         <v>45078</v>
@@ -23064,7 +23064,7 @@
     </row>
     <row r="731">
       <c r="A731" s="1" t="n">
-        <v>965</v>
+        <v>85</v>
       </c>
       <c r="B731" s="2" t="n">
         <v>45079</v>
@@ -23498,7 +23498,7 @@
     </row>
     <row r="745">
       <c r="A745" s="1" t="n">
-        <v>964</v>
+        <v>84</v>
       </c>
       <c r="B745" s="2" t="n">
         <v>45082</v>
@@ -23653,7 +23653,7 @@
     </row>
     <row r="750">
       <c r="A750" s="1" t="n">
-        <v>963</v>
+        <v>83</v>
       </c>
       <c r="B750" s="2" t="n">
         <v>45084</v>
@@ -23684,7 +23684,7 @@
     </row>
     <row r="751">
       <c r="A751" s="1" t="n">
-        <v>962</v>
+        <v>82</v>
       </c>
       <c r="B751" s="2" t="n">
         <v>45084</v>
@@ -23715,7 +23715,7 @@
     </row>
     <row r="752">
       <c r="A752" s="1" t="n">
-        <v>961</v>
+        <v>81</v>
       </c>
       <c r="B752" s="2" t="n">
         <v>45085</v>
@@ -24087,7 +24087,7 @@
     </row>
     <row r="764">
       <c r="A764" s="1" t="n">
-        <v>960</v>
+        <v>80</v>
       </c>
       <c r="B764" s="2" t="n">
         <v>45086</v>
@@ -24118,7 +24118,7 @@
     </row>
     <row r="765">
       <c r="A765" s="1" t="n">
-        <v>959</v>
+        <v>79</v>
       </c>
       <c r="B765" s="2" t="n">
         <v>45087</v>
@@ -24149,7 +24149,7 @@
     </row>
     <row r="766">
       <c r="A766" s="1" t="n">
-        <v>958</v>
+        <v>78</v>
       </c>
       <c r="B766" s="2" t="n">
         <v>45087</v>
@@ -24242,7 +24242,7 @@
     </row>
     <row r="769">
       <c r="A769" s="1" t="n">
-        <v>957</v>
+        <v>77</v>
       </c>
       <c r="B769" s="2" t="n">
         <v>45088</v>
@@ -24273,7 +24273,7 @@
     </row>
     <row r="770">
       <c r="A770" s="1" t="n">
-        <v>956</v>
+        <v>76</v>
       </c>
       <c r="B770" s="2" t="n">
         <v>45089</v>
@@ -24304,7 +24304,7 @@
     </row>
     <row r="771">
       <c r="A771" s="1" t="n">
-        <v>955</v>
+        <v>75</v>
       </c>
       <c r="B771" s="2" t="n">
         <v>45089</v>
@@ -24335,7 +24335,7 @@
     </row>
     <row r="772">
       <c r="A772" s="1" t="n">
-        <v>954</v>
+        <v>74</v>
       </c>
       <c r="B772" s="2" t="n">
         <v>45089</v>
@@ -24459,7 +24459,7 @@
     </row>
     <row r="776">
       <c r="A776" s="1" t="n">
-        <v>953</v>
+        <v>73</v>
       </c>
       <c r="B776" s="2" t="n">
         <v>45090</v>
@@ -25017,7 +25017,7 @@
     </row>
     <row r="794">
       <c r="A794" s="1" t="n">
-        <v>952</v>
+        <v>72</v>
       </c>
       <c r="B794" s="2" t="n">
         <v>45092</v>
@@ -25389,7 +25389,7 @@
     </row>
     <row r="806">
       <c r="A806" s="1" t="n">
-        <v>951</v>
+        <v>71</v>
       </c>
       <c r="B806" s="2" t="n">
         <v>45093</v>
@@ -25420,7 +25420,7 @@
     </row>
     <row r="807">
       <c r="A807" s="1" t="n">
-        <v>950</v>
+        <v>70</v>
       </c>
       <c r="B807" s="2" t="n">
         <v>45093</v>
@@ -25451,7 +25451,7 @@
     </row>
     <row r="808">
       <c r="A808" s="1" t="n">
-        <v>949</v>
+        <v>69</v>
       </c>
       <c r="B808" s="2" t="n">
         <v>45093</v>
@@ -25885,7 +25885,7 @@
     </row>
     <row r="822">
       <c r="A822" s="1" t="n">
-        <v>948</v>
+        <v>68</v>
       </c>
       <c r="B822" s="2" t="n">
         <v>45096</v>
@@ -25916,7 +25916,7 @@
     </row>
     <row r="823">
       <c r="A823" s="1" t="n">
-        <v>946</v>
+        <v>66</v>
       </c>
       <c r="B823" s="2" t="n">
         <v>45096</v>
@@ -25947,7 +25947,7 @@
     </row>
     <row r="824">
       <c r="A824" s="1" t="n">
-        <v>947</v>
+        <v>67</v>
       </c>
       <c r="B824" s="2" t="n">
         <v>45096</v>
@@ -26071,7 +26071,7 @@
     </row>
     <row r="828">
       <c r="A828" s="1" t="n">
-        <v>945</v>
+        <v>65</v>
       </c>
       <c r="B828" s="2" t="n">
         <v>45097</v>
@@ -26133,7 +26133,7 @@
     </row>
     <row r="830">
       <c r="A830" s="1" t="n">
-        <v>944</v>
+        <v>64</v>
       </c>
       <c r="B830" s="2" t="n">
         <v>45098</v>
@@ -26164,7 +26164,7 @@
     </row>
     <row r="831">
       <c r="A831" s="1" t="n">
-        <v>943</v>
+        <v>63</v>
       </c>
       <c r="B831" s="2" t="n">
         <v>45098</v>
@@ -26195,7 +26195,7 @@
     </row>
     <row r="832">
       <c r="A832" s="1" t="n">
-        <v>940</v>
+        <v>60</v>
       </c>
       <c r="B832" s="2" t="n">
         <v>45098</v>
@@ -26257,7 +26257,7 @@
     </row>
     <row r="834">
       <c r="A834" s="1" t="n">
-        <v>942</v>
+        <v>62</v>
       </c>
       <c r="B834" s="2" t="n">
         <v>45099</v>
@@ -26288,7 +26288,7 @@
     </row>
     <row r="835">
       <c r="A835" s="1" t="n">
-        <v>941</v>
+        <v>61</v>
       </c>
       <c r="B835" s="2" t="n">
         <v>45099</v>
@@ -26722,7 +26722,7 @@
     </row>
     <row r="849">
       <c r="A849" s="1" t="n">
-        <v>938</v>
+        <v>58</v>
       </c>
       <c r="B849" s="2" t="n">
         <v>45103</v>
@@ -26753,7 +26753,7 @@
     </row>
     <row r="850">
       <c r="A850" s="1" t="n">
-        <v>939</v>
+        <v>59</v>
       </c>
       <c r="B850" s="2" t="n">
         <v>45103</v>
@@ -27001,7 +27001,7 @@
     </row>
     <row r="858">
       <c r="A858" s="1" t="n">
-        <v>937</v>
+        <v>57</v>
       </c>
       <c r="B858" s="2" t="n">
         <v>45103</v>
@@ -27032,7 +27032,7 @@
     </row>
     <row r="859">
       <c r="A859" s="1" t="n">
-        <v>936</v>
+        <v>56</v>
       </c>
       <c r="B859" s="2" t="n">
         <v>45104</v>
@@ -27218,7 +27218,7 @@
     </row>
     <row r="865">
       <c r="A865" s="1" t="n">
-        <v>935</v>
+        <v>55</v>
       </c>
       <c r="B865" s="2" t="n">
         <v>45105</v>
@@ -27404,7 +27404,7 @@
     </row>
     <row r="871">
       <c r="A871" s="1" t="n">
-        <v>930</v>
+        <v>50</v>
       </c>
       <c r="B871" s="2" t="n">
         <v>45106</v>
@@ -27435,7 +27435,7 @@
     </row>
     <row r="872">
       <c r="A872" s="1" t="n">
-        <v>929</v>
+        <v>49</v>
       </c>
       <c r="B872" s="2" t="n">
         <v>45106</v>
@@ -27528,7 +27528,7 @@
     </row>
     <row r="875">
       <c r="A875" s="1" t="n">
-        <v>934</v>
+        <v>54</v>
       </c>
       <c r="B875" s="2" t="n">
         <v>45107</v>
@@ -27559,7 +27559,7 @@
     </row>
     <row r="876">
       <c r="A876" s="1" t="n">
-        <v>933</v>
+        <v>53</v>
       </c>
       <c r="B876" s="2" t="n">
         <v>45107</v>
@@ -27590,7 +27590,7 @@
     </row>
     <row r="877">
       <c r="A877" s="1" t="n">
-        <v>932</v>
+        <v>52</v>
       </c>
       <c r="B877" s="2" t="n">
         <v>45107</v>
@@ -27621,7 +27621,7 @@
     </row>
     <row r="878">
       <c r="A878" s="1" t="n">
-        <v>931</v>
+        <v>51</v>
       </c>
       <c r="B878" s="2" t="n">
         <v>45107</v>
@@ -27807,7 +27807,7 @@
     </row>
     <row r="884">
       <c r="A884" s="1" t="n">
-        <v>928</v>
+        <v>48</v>
       </c>
       <c r="B884" s="2" t="n">
         <v>45110</v>
@@ -28086,7 +28086,7 @@
     </row>
     <row r="893">
       <c r="A893" s="1" t="n">
-        <v>926</v>
+        <v>46</v>
       </c>
       <c r="B893" s="2" t="n">
         <v>45110</v>
@@ -28117,7 +28117,7 @@
     </row>
     <row r="894">
       <c r="A894" s="1" t="n">
-        <v>927</v>
+        <v>47</v>
       </c>
       <c r="B894" s="2" t="n">
         <v>45110</v>
@@ -28365,7 +28365,7 @@
     </row>
     <row r="902">
       <c r="A902" s="1" t="n">
-        <v>924</v>
+        <v>44</v>
       </c>
       <c r="B902" s="2" t="n">
         <v>45113</v>
@@ -28396,7 +28396,7 @@
     </row>
     <row r="903">
       <c r="A903" s="1" t="n">
-        <v>925</v>
+        <v>45</v>
       </c>
       <c r="B903" s="2" t="n">
         <v>45113</v>
@@ -28582,7 +28582,7 @@
     </row>
     <row r="909">
       <c r="A909" s="1" t="n">
-        <v>923</v>
+        <v>43</v>
       </c>
       <c r="B909" s="2" t="n">
         <v>45115</v>
@@ -28923,7 +28923,7 @@
     </row>
     <row r="920">
       <c r="A920" s="1" t="n">
-        <v>918</v>
+        <v>38</v>
       </c>
       <c r="B920" s="2" t="n">
         <v>45118</v>
@@ -28954,7 +28954,7 @@
     </row>
     <row r="921">
       <c r="A921" s="1" t="n">
-        <v>921</v>
+        <v>41</v>
       </c>
       <c r="B921" s="2" t="n">
         <v>45118</v>
@@ -28985,7 +28985,7 @@
     </row>
     <row r="922">
       <c r="A922" s="1" t="n">
-        <v>922</v>
+        <v>42</v>
       </c>
       <c r="B922" s="2" t="n">
         <v>45118</v>
@@ -29171,7 +29171,7 @@
     </row>
     <row r="928">
       <c r="A928" s="1" t="n">
-        <v>920</v>
+        <v>40</v>
       </c>
       <c r="B928" s="2" t="n">
         <v>45119</v>
@@ -29202,7 +29202,7 @@
     </row>
     <row r="929">
       <c r="A929" s="1" t="n">
-        <v>919</v>
+        <v>39</v>
       </c>
       <c r="B929" s="2" t="n">
         <v>45119</v>
@@ -29574,7 +29574,7 @@
     </row>
     <row r="941">
       <c r="A941" s="1" t="n">
-        <v>917</v>
+        <v>37</v>
       </c>
       <c r="B941" s="2" t="n">
         <v>45123</v>
@@ -29822,7 +29822,7 @@
     </row>
     <row r="949">
       <c r="A949" s="1" t="n">
-        <v>915</v>
+        <v>35</v>
       </c>
       <c r="B949" s="2" t="n">
         <v>45124</v>
@@ -29853,7 +29853,7 @@
     </row>
     <row r="950">
       <c r="A950" s="1" t="n">
-        <v>916</v>
+        <v>36</v>
       </c>
       <c r="B950" s="2" t="n">
         <v>45124</v>
@@ -29946,7 +29946,7 @@
     </row>
     <row r="953">
       <c r="A953" s="1" t="n">
-        <v>913</v>
+        <v>33</v>
       </c>
       <c r="B953" s="2" t="n">
         <v>45126</v>
@@ -30132,7 +30132,7 @@
     </row>
     <row r="959">
       <c r="A959" s="1" t="n">
-        <v>914</v>
+        <v>34</v>
       </c>
       <c r="B959" s="2" t="n">
         <v>45126</v>
@@ -30194,7 +30194,7 @@
     </row>
     <row r="961">
       <c r="A961" s="1" t="n">
-        <v>911</v>
+        <v>31</v>
       </c>
       <c r="B961" s="2" t="n">
         <v>45128</v>
@@ -30256,7 +30256,7 @@
     </row>
     <row r="963">
       <c r="A963" s="1" t="n">
-        <v>912</v>
+        <v>32</v>
       </c>
       <c r="B963" s="2" t="n">
         <v>45129</v>
@@ -30349,7 +30349,7 @@
     </row>
     <row r="966">
       <c r="A966" s="1" t="n">
-        <v>910</v>
+        <v>30</v>
       </c>
       <c r="B966" s="2" t="n">
         <v>45131</v>
@@ -30628,7 +30628,7 @@
     </row>
     <row r="975">
       <c r="A975" s="1" t="n">
-        <v>908</v>
+        <v>28</v>
       </c>
       <c r="B975" s="2" t="n">
         <v>45133</v>
@@ -30659,7 +30659,7 @@
     </row>
     <row r="976">
       <c r="A976" s="1" t="n">
-        <v>907</v>
+        <v>27</v>
       </c>
       <c r="B976" s="2" t="n">
         <v>45133</v>
@@ -30690,7 +30690,7 @@
     </row>
     <row r="977">
       <c r="A977" s="1" t="n">
-        <v>906</v>
+        <v>26</v>
       </c>
       <c r="B977" s="2" t="n">
         <v>45133</v>
@@ -30907,7 +30907,7 @@
     </row>
     <row r="984">
       <c r="A984" s="1" t="n">
-        <v>909</v>
+        <v>29</v>
       </c>
       <c r="B984" s="2" t="n">
         <v>45133</v>
@@ -30938,7 +30938,7 @@
     </row>
     <row r="985">
       <c r="A985" s="1" t="n">
-        <v>905</v>
+        <v>25</v>
       </c>
       <c r="B985" s="2" t="n">
         <v>45134</v>
@@ -30969,7 +30969,7 @@
     </row>
     <row r="986">
       <c r="A986" s="1" t="n">
-        <v>904</v>
+        <v>24</v>
       </c>
       <c r="B986" s="2" t="n">
         <v>45134</v>
@@ -31310,7 +31310,7 @@
     </row>
     <row r="997">
       <c r="A997" s="1" t="n">
-        <v>901</v>
+        <v>21</v>
       </c>
       <c r="B997" s="2" t="n">
         <v>45135</v>
@@ -31341,7 +31341,7 @@
     </row>
     <row r="998">
       <c r="A998" s="1" t="n">
-        <v>902</v>
+        <v>22</v>
       </c>
       <c r="B998" s="2" t="n">
         <v>45135</v>
@@ -31372,7 +31372,7 @@
     </row>
     <row r="999">
       <c r="A999" s="1" t="n">
-        <v>903</v>
+        <v>23</v>
       </c>
       <c r="B999" s="2" t="n">
         <v>45135</v>
@@ -31744,7 +31744,7 @@
     </row>
     <row r="1011">
       <c r="A1011" s="1" t="n">
-        <v>900</v>
+        <v>20</v>
       </c>
       <c r="B1011" s="2" t="n">
         <v>45138</v>
@@ -31775,7 +31775,7 @@
     </row>
     <row r="1012">
       <c r="A1012" s="1" t="n">
-        <v>899</v>
+        <v>19</v>
       </c>
       <c r="B1012" s="2" t="n">
         <v>45138</v>
@@ -31837,7 +31837,7 @@
     </row>
     <row r="1014">
       <c r="A1014" s="1" t="n">
-        <v>897</v>
+        <v>17</v>
       </c>
       <c r="B1014" s="2" t="n">
         <v>45139</v>
@@ -31868,7 +31868,7 @@
     </row>
     <row r="1015">
       <c r="A1015" s="1" t="n">
-        <v>898</v>
+        <v>18</v>
       </c>
       <c r="B1015" s="2" t="n">
         <v>45139</v>
@@ -32426,7 +32426,7 @@
     </row>
     <row r="1033">
       <c r="A1033" s="1" t="n">
-        <v>896</v>
+        <v>16</v>
       </c>
       <c r="B1033" s="2" t="n">
         <v>45143</v>
@@ -32457,7 +32457,7 @@
     </row>
     <row r="1034">
       <c r="A1034" s="1" t="n">
-        <v>895</v>
+        <v>15</v>
       </c>
       <c r="B1034" s="2" t="n">
         <v>45143</v>
@@ -32829,7 +32829,7 @@
     </row>
     <row r="1046">
       <c r="A1046" s="1" t="n">
-        <v>894</v>
+        <v>14</v>
       </c>
       <c r="B1046" s="2" t="n">
         <v>45147</v>
@@ -32860,7 +32860,7 @@
     </row>
     <row r="1047">
       <c r="A1047" s="1" t="n">
-        <v>893</v>
+        <v>13</v>
       </c>
       <c r="B1047" s="2" t="n">
         <v>45147</v>
@@ -34007,7 +34007,7 @@
     </row>
     <row r="1084">
       <c r="A1084" s="1" t="n">
-        <v>891</v>
+        <v>11</v>
       </c>
       <c r="B1084" s="2" t="n">
         <v>45160</v>
@@ -34162,7 +34162,7 @@
     </row>
     <row r="1089">
       <c r="A1089" s="1" t="n">
-        <v>892</v>
+        <v>12</v>
       </c>
       <c r="B1089" s="2" t="n">
         <v>45162</v>
@@ -34193,7 +34193,7 @@
     </row>
     <row r="1090">
       <c r="A1090" s="1" t="n">
-        <v>890</v>
+        <v>10</v>
       </c>
       <c r="B1090" s="2" t="n">
         <v>45162</v>
@@ -34224,7 +34224,7 @@
     </row>
     <row r="1091">
       <c r="A1091" s="1" t="n">
-        <v>889</v>
+        <v>9</v>
       </c>
       <c r="B1091" s="2" t="n">
         <v>45162</v>
@@ -34503,7 +34503,7 @@
     </row>
     <row r="1100">
       <c r="A1100" s="1" t="n">
-        <v>887</v>
+        <v>7</v>
       </c>
       <c r="B1100" s="2" t="n">
         <v>45163</v>
@@ -34534,7 +34534,7 @@
     </row>
     <row r="1101">
       <c r="A1101" s="1" t="n">
-        <v>888</v>
+        <v>8</v>
       </c>
       <c r="B1101" s="2" t="n">
         <v>45163</v>
@@ -34689,7 +34689,7 @@
     </row>
     <row r="1106">
       <c r="A1106" s="1" t="n">
-        <v>886</v>
+        <v>6</v>
       </c>
       <c r="B1106" s="2" t="n">
         <v>45165</v>
@@ -34782,7 +34782,7 @@
     </row>
     <row r="1109">
       <c r="A1109" s="1" t="n">
-        <v>882</v>
+        <v>2</v>
       </c>
       <c r="B1109" s="2" t="n">
         <v>45166</v>
@@ -34999,7 +34999,7 @@
     </row>
     <row r="1116">
       <c r="A1116" s="1" t="n">
-        <v>885</v>
+        <v>5</v>
       </c>
       <c r="B1116" s="2" t="n">
         <v>45166</v>
@@ -35030,7 +35030,7 @@
     </row>
     <row r="1117">
       <c r="A1117" s="1" t="n">
-        <v>884</v>
+        <v>4</v>
       </c>
       <c r="B1117" s="2" t="n">
         <v>45166</v>
@@ -35061,7 +35061,7 @@
     </row>
     <row r="1118">
       <c r="A1118" s="1" t="n">
-        <v>883</v>
+        <v>3</v>
       </c>
       <c r="B1118" s="2" t="n">
         <v>45166</v>
@@ -35619,7 +35619,7 @@
     </row>
     <row r="1136">
       <c r="A1136" s="1" t="n">
-        <v>880</v>
+        <v>0</v>
       </c>
       <c r="B1136" s="2" t="n">
         <v>45169</v>
@@ -35650,7 +35650,7 @@
     </row>
     <row r="1137">
       <c r="A1137" s="1" t="n">
-        <v>881</v>
+        <v>1</v>
       </c>
       <c r="B1137" s="2" t="n">
         <v>45169</v>

</xml_diff>